<commit_message>
small optimization a cross the code
</commit_message>
<xml_diff>
--- a/test data/graph.xlsx
+++ b/test data/graph.xlsx
@@ -1,48 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Click\Documents\Graphite\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B20BC43-0064-4CB5-A696-D66FCB8E7400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="3765" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>graph</t>
-  </si>
-  <si>
-    <t>yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -56,11 +45,11 @@
   </fills>
   <borders count="2">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
@@ -75,15 +64,15 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -91,19 +80,16 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
@@ -149,13 +135,13 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Thai" typeface="Angsana New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -183,13 +169,13 @@
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Thai" typeface="Cordia New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -386,123 +372,299 @@
 </a:theme>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle"/>
+        </a:gradFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>2345</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>8568</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>6578</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>5677</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>4893</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
   </sheetData>
+  <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
work sheet now is better
</commit_message>
<xml_diff>
--- a/test data/graph.xlsx
+++ b/test data/graph.xlsx
@@ -2,20 +2,24 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
     <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>graph</t>
+  </si>
+  <si>
+    <t>line</t>
   </si>
 </sst>
 </file>
@@ -31,8 +35,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11.000000"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -53,16 +55,16 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color theme="1"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color theme="1"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color theme="1"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color theme="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
@@ -71,8 +73,8 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0"/>
+    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="0" pivotButton="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -583,82 +585,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+  </sheetPr>
   <sheetViews>
     <sheetView zoomScale="100" workbookViewId="0">
-      <selection activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7">
+        <v>12</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8">
+        <v>14</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9">
+        <v>16</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10">
+        <v>18</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12">
+        <v>22</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13">
+        <v>24</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14">
         <v>13</v>
+      </c>
+      <c r="B14">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>